<commit_message>
>implementazione rule empty >adattamento al require_once di Data.php
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">nome </t>
   </si>
@@ -41,15 +41,12 @@
   <si>
     <t xml:space="preserve">codice fiscale </t>
   </si>
-  <si>
-    <t>MRNRRT94H26F471X</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +97,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -146,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,9 +183,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,6 +218,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,21 +394,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -430,9 +437,6 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -440,17 +444,17 @@
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -458,12 +462,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
[1.1.c] Regola: controllo nazione
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">nome </t>
   </si>
@@ -52,13 +52,22 @@
   </si>
   <si>
     <t>aaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Calimera</t>
+  </si>
+  <si>
+    <t>nazione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,7 +172,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,9 +204,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,6 +239,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,21 +415,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +445,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -448,8 +462,11 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -464,6 +481,9 @@
       </c>
       <c r="E3" t="s">
         <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -476,12 +496,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -489,12 +509,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>